<commit_message>
Modulo 1 y 2 (test)
</commit_message>
<xml_diff>
--- a/input/factores_bc.xlsx
+++ b/input/factores_bc.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaz/Documents/STEP_3/copert5App/copert_5/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ignaz/Documents/STEP_3/copert5App/copert_5.nosync/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A777255A-2793-5043-9FBF-7A33AFEBBDEC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E241C3F-782F-D945-ADCF-E350285AA015}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12800" yWindow="0" windowWidth="14400" windowHeight="18000" xr2:uid="{11B744EB-CB34-1A4B-9C51-F35778FB4385}"/>
   </bookViews>
@@ -444,7 +444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F23B3295-9DEC-D540-9533-C41943823C49}">
   <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
       <selection activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>

</xml_diff>